<commit_message>
Sayfa2 Eklendi (devam ediyor)
</commit_message>
<xml_diff>
--- a/Sorular.xlsx
+++ b/Sorular.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet\OneDrive\Masaüstü\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet\OneDrive\Masaüstü\Yeni klasör\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96B627C8-59B0-4EDE-B3C3-E8330774C662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9706D5C-AE4D-4509-8216-20258B8030DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="2250" windowWidth="15375" windowHeight="7995" xr2:uid="{BCF4A1DB-2C43-4542-B577-DEE48766ECF3}"/>
+    <workbookView xWindow="4770" yWindow="2250" windowWidth="15375" windowHeight="7995" activeTab="1" xr2:uid="{BCF4A1DB-2C43-4542-B577-DEE48766ECF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Normal Sorular</t>
   </si>
@@ -99,6 +100,66 @@
   </si>
   <si>
     <t>z10</t>
+  </si>
+  <si>
+    <t>n1s2</t>
+  </si>
+  <si>
+    <t>n2s2</t>
+  </si>
+  <si>
+    <t>n3s2</t>
+  </si>
+  <si>
+    <t>n4s2</t>
+  </si>
+  <si>
+    <t>n5s2</t>
+  </si>
+  <si>
+    <t>n6s2</t>
+  </si>
+  <si>
+    <t>n7s2</t>
+  </si>
+  <si>
+    <t>n8s2</t>
+  </si>
+  <si>
+    <t>n9s2</t>
+  </si>
+  <si>
+    <t>n10s2</t>
+  </si>
+  <si>
+    <t>z1s2</t>
+  </si>
+  <si>
+    <t>z2s2</t>
+  </si>
+  <si>
+    <t>z3s2</t>
+  </si>
+  <si>
+    <t>z4s2</t>
+  </si>
+  <si>
+    <t>z5s2</t>
+  </si>
+  <si>
+    <t>z6s2</t>
+  </si>
+  <si>
+    <t>z7s2</t>
+  </si>
+  <si>
+    <t>z8s2</t>
+  </si>
+  <si>
+    <t>z9s2</t>
+  </si>
+  <si>
+    <t>z10s2</t>
   </si>
 </sst>
 </file>
@@ -463,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E9C376-7B9A-451F-94B8-CB34E5F98680}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,4 +626,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB27BB5-7F44-4D51-A431-9DDBD9A4EF0D}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Yeni Versiyon hacked by halim
</commit_message>
<xml_diff>
--- a/Sorular.xlsx
+++ b/Sorular.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\SoruUygulamasi-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0961A30E-116E-4E7C-9D0B-F298070B10A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6803FCA9-796F-4EEC-B1FB-2756E45791BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31995" yWindow="825" windowWidth="15810" windowHeight="11385" activeTab="2" xr2:uid="{BCF4A1DB-2C43-4542-B577-DEE48766ECF3}"/>
+    <workbookView xWindow="3555" yWindow="1605" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{BCF4A1DB-2C43-4542-B577-DEE48766ECF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="212">
   <si>
     <t>Normal Sorular</t>
   </si>
@@ -191,6 +191,486 @@
   </si>
   <si>
     <t>z5s3</t>
+  </si>
+  <si>
+    <t>n11</t>
+  </si>
+  <si>
+    <t>z11</t>
+  </si>
+  <si>
+    <t>n12</t>
+  </si>
+  <si>
+    <t>z12</t>
+  </si>
+  <si>
+    <t>n13</t>
+  </si>
+  <si>
+    <t>z13</t>
+  </si>
+  <si>
+    <t>n14</t>
+  </si>
+  <si>
+    <t>z14</t>
+  </si>
+  <si>
+    <t>n15</t>
+  </si>
+  <si>
+    <t>z15</t>
+  </si>
+  <si>
+    <t>n16</t>
+  </si>
+  <si>
+    <t>z16</t>
+  </si>
+  <si>
+    <t>n17</t>
+  </si>
+  <si>
+    <t>z17</t>
+  </si>
+  <si>
+    <t>n18</t>
+  </si>
+  <si>
+    <t>z18</t>
+  </si>
+  <si>
+    <t>n19</t>
+  </si>
+  <si>
+    <t>z19</t>
+  </si>
+  <si>
+    <t>n20</t>
+  </si>
+  <si>
+    <t>z20</t>
+  </si>
+  <si>
+    <t>n21</t>
+  </si>
+  <si>
+    <t>z21</t>
+  </si>
+  <si>
+    <t>n22</t>
+  </si>
+  <si>
+    <t>z22</t>
+  </si>
+  <si>
+    <t>n23</t>
+  </si>
+  <si>
+    <t>z23</t>
+  </si>
+  <si>
+    <t>n24</t>
+  </si>
+  <si>
+    <t>z24</t>
+  </si>
+  <si>
+    <t>n25</t>
+  </si>
+  <si>
+    <t>z25</t>
+  </si>
+  <si>
+    <t>n26</t>
+  </si>
+  <si>
+    <t>z26</t>
+  </si>
+  <si>
+    <t>n27</t>
+  </si>
+  <si>
+    <t>z27</t>
+  </si>
+  <si>
+    <t>n28</t>
+  </si>
+  <si>
+    <t>z28</t>
+  </si>
+  <si>
+    <t>n29</t>
+  </si>
+  <si>
+    <t>z29</t>
+  </si>
+  <si>
+    <t>n30</t>
+  </si>
+  <si>
+    <t>z30</t>
+  </si>
+  <si>
+    <t>n31</t>
+  </si>
+  <si>
+    <t>z31</t>
+  </si>
+  <si>
+    <t>n32</t>
+  </si>
+  <si>
+    <t>z32</t>
+  </si>
+  <si>
+    <t>n33</t>
+  </si>
+  <si>
+    <t>z33</t>
+  </si>
+  <si>
+    <t>n34</t>
+  </si>
+  <si>
+    <t>z34</t>
+  </si>
+  <si>
+    <t>n35</t>
+  </si>
+  <si>
+    <t>z35</t>
+  </si>
+  <si>
+    <t>n36</t>
+  </si>
+  <si>
+    <t>z36</t>
+  </si>
+  <si>
+    <t>n37</t>
+  </si>
+  <si>
+    <t>z37</t>
+  </si>
+  <si>
+    <t>n38</t>
+  </si>
+  <si>
+    <t>z38</t>
+  </si>
+  <si>
+    <t>n39</t>
+  </si>
+  <si>
+    <t>z39</t>
+  </si>
+  <si>
+    <t>n40</t>
+  </si>
+  <si>
+    <t>z40</t>
+  </si>
+  <si>
+    <t>n6s3</t>
+  </si>
+  <si>
+    <t>z6s3</t>
+  </si>
+  <si>
+    <t>n7s3</t>
+  </si>
+  <si>
+    <t>z7s3</t>
+  </si>
+  <si>
+    <t>n8s3</t>
+  </si>
+  <si>
+    <t>z8s3</t>
+  </si>
+  <si>
+    <t>n9s3</t>
+  </si>
+  <si>
+    <t>z9s3</t>
+  </si>
+  <si>
+    <t>n10s3</t>
+  </si>
+  <si>
+    <t>z10s3</t>
+  </si>
+  <si>
+    <t>n1s4</t>
+  </si>
+  <si>
+    <t>z1s4</t>
+  </si>
+  <si>
+    <t>n2s4</t>
+  </si>
+  <si>
+    <t>z2s4</t>
+  </si>
+  <si>
+    <t>n3s4</t>
+  </si>
+  <si>
+    <t>z3s4</t>
+  </si>
+  <si>
+    <t>n4s4</t>
+  </si>
+  <si>
+    <t>z4s4</t>
+  </si>
+  <si>
+    <t>n5s4</t>
+  </si>
+  <si>
+    <t>z5s4</t>
+  </si>
+  <si>
+    <t>n6s4</t>
+  </si>
+  <si>
+    <t>z6s4</t>
+  </si>
+  <si>
+    <t>n7s4</t>
+  </si>
+  <si>
+    <t>z7s4</t>
+  </si>
+  <si>
+    <t>n8s4</t>
+  </si>
+  <si>
+    <t>z8s4</t>
+  </si>
+  <si>
+    <t>n9s4</t>
+  </si>
+  <si>
+    <t>z9s4</t>
+  </si>
+  <si>
+    <t>n10s4</t>
+  </si>
+  <si>
+    <t>z10s4</t>
+  </si>
+  <si>
+    <t>n1s5</t>
+  </si>
+  <si>
+    <t>z1s5</t>
+  </si>
+  <si>
+    <t>n2s5</t>
+  </si>
+  <si>
+    <t>z2s5</t>
+  </si>
+  <si>
+    <t>n3s5</t>
+  </si>
+  <si>
+    <t>z3s5</t>
+  </si>
+  <si>
+    <t>n4s5</t>
+  </si>
+  <si>
+    <t>z4s5</t>
+  </si>
+  <si>
+    <t>n5s5</t>
+  </si>
+  <si>
+    <t>z5s5</t>
+  </si>
+  <si>
+    <t>n6s5</t>
+  </si>
+  <si>
+    <t>z6s5</t>
+  </si>
+  <si>
+    <t>n7s5</t>
+  </si>
+  <si>
+    <t>z7s5</t>
+  </si>
+  <si>
+    <t>n8s5</t>
+  </si>
+  <si>
+    <t>z8s5</t>
+  </si>
+  <si>
+    <t>n9s5</t>
+  </si>
+  <si>
+    <t>z9s5</t>
+  </si>
+  <si>
+    <t>n10s5</t>
+  </si>
+  <si>
+    <t>z10s5</t>
+  </si>
+  <si>
+    <t>n1s6</t>
+  </si>
+  <si>
+    <t>z1s6</t>
+  </si>
+  <si>
+    <t>n2s6</t>
+  </si>
+  <si>
+    <t>z2s6</t>
+  </si>
+  <si>
+    <t>n3s6</t>
+  </si>
+  <si>
+    <t>z3s6</t>
+  </si>
+  <si>
+    <t>n4s6</t>
+  </si>
+  <si>
+    <t>z4s6</t>
+  </si>
+  <si>
+    <t>n5s6</t>
+  </si>
+  <si>
+    <t>z5s6</t>
+  </si>
+  <si>
+    <t>n1s7</t>
+  </si>
+  <si>
+    <t>z1s7</t>
+  </si>
+  <si>
+    <t>n2s7</t>
+  </si>
+  <si>
+    <t>z2s7</t>
+  </si>
+  <si>
+    <t>n3s7</t>
+  </si>
+  <si>
+    <t>z3s7</t>
+  </si>
+  <si>
+    <t>n4s7</t>
+  </si>
+  <si>
+    <t>z4s7</t>
+  </si>
+  <si>
+    <t>n5s7</t>
+  </si>
+  <si>
+    <t>z5s7</t>
+  </si>
+  <si>
+    <t>n1s8</t>
+  </si>
+  <si>
+    <t>z1s8</t>
+  </si>
+  <si>
+    <t>n2s8</t>
+  </si>
+  <si>
+    <t>z2s8</t>
+  </si>
+  <si>
+    <t>n3s8</t>
+  </si>
+  <si>
+    <t>z3s8</t>
+  </si>
+  <si>
+    <t>n4s8</t>
+  </si>
+  <si>
+    <t>z4s8</t>
+  </si>
+  <si>
+    <t>n5s8</t>
+  </si>
+  <si>
+    <t>z5s8</t>
+  </si>
+  <si>
+    <t>n1s9</t>
+  </si>
+  <si>
+    <t>z1s9</t>
+  </si>
+  <si>
+    <t>n2s9</t>
+  </si>
+  <si>
+    <t>z2s9</t>
+  </si>
+  <si>
+    <t>n3s9</t>
+  </si>
+  <si>
+    <t>z3s9</t>
+  </si>
+  <si>
+    <t>n4s9</t>
+  </si>
+  <si>
+    <t>z4s9</t>
+  </si>
+  <si>
+    <t>n5s9</t>
+  </si>
+  <si>
+    <t>z5s9</t>
+  </si>
+  <si>
+    <t>n1s10</t>
+  </si>
+  <si>
+    <t>z1s10</t>
+  </si>
+  <si>
+    <t>n2s10</t>
+  </si>
+  <si>
+    <t>z2s10</t>
+  </si>
+  <si>
+    <t>n3s10</t>
+  </si>
+  <si>
+    <t>z3s10</t>
+  </si>
+  <si>
+    <t>n4s10</t>
+  </si>
+  <si>
+    <t>z4s10</t>
+  </si>
+  <si>
+    <t>n5s10</t>
+  </si>
+  <si>
+    <t>z5s10</t>
   </si>
 </sst>
 </file>
@@ -560,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E9C376-7B9A-451F-94B8-CB34E5F98680}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +1140,248 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -668,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB27BB5-7F44-4D51-A431-9DDBD9A4EF0D}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,17 +1489,258 @@
         <v>41</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C079D31D-4BBD-46F8-9908-75EA3514376C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +1797,286 @@
         <v>51</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>204</v>
+      </c>
+      <c r="B38" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>210</v>
+      </c>
+      <c r="B41" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>